<commit_message>
Implement the Excel Import Feature
</commit_message>
<xml_diff>
--- a/ScheduleJobDesktop/Resources/EventConfigTemplate.xlsx
+++ b/ScheduleJobDesktop/Resources/EventConfigTemplate.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>EventDate</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>事件名称2</t>
+  </si>
+  <si>
+    <t>1058A90</t>
+  </si>
+  <si>
+    <t>1058B68</t>
+  </si>
+  <si>
+    <t>EventId：采用16进制</t>
   </si>
 </sst>
 </file>
@@ -57,7 +66,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -67,6 +76,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -98,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -112,6 +127,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,50 +411,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>42718.527083333334</v>
+      <c r="A2" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
-        <v>17140368</v>
+      <c r="C2" s="2">
+        <v>42718.527083333334</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>42705.981944444444</v>
+      <c r="A3" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
-        <v>17140584</v>
+      <c r="C3" s="4">
+        <v>42705.981944444444</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -445,9 +463,9 @@
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="5"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -478,6 +496,13 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>